<commit_message>
first commit of 2018
</commit_message>
<xml_diff>
--- a/main/static/records/poc.xlsx
+++ b/main/static/records/poc.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t xml:space="preserve">09176214704</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t xml:space="preserve">Alsons Trading Acct#: ACCT-ABL4971, DueDate: 9/03, Amt.Overdue: 12,418.00, No.of mos Overdue: 2, Outs.Bal: 11,180.00.For details call:056 4111141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">639159484200</t>
   </si>
 </sst>
 </file>
@@ -128,7 +131,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -156,22 +159,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -194,63 +181,59 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normale 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normale 3" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normale 4" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normale 5" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normale 6" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -323,21 +306,21 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="189.813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.3846153846154"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="191.53036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -389,9 +372,13 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -504,7 +491,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -530,7 +517,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>